<commit_message>
Added a more precice time measurement.
</commit_message>
<xml_diff>
--- a/STM32G030K6T6/ControlHub/DefectList.xlsx
+++ b/STM32G030K6T6/ControlHub/DefectList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dagak\GitHub\stm32\STM32G030K6T6\ControlHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598ED557-7303-49CC-8101-9D2CF1579BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0B68FA-2005-43B5-9D57-C0491250E7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="735" windowWidth="33480" windowHeight="18705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41250" yWindow="2850" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Defects" sheetId="1" r:id="rId1"/>
+    <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Defect-ID</t>
   </si>
@@ -44,13 +45,40 @@
   </si>
   <si>
     <t>Build</t>
+  </si>
+  <si>
+    <t>Stop watch not stopping when all targets have been hit</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Target cover to servo attachment is still weak. May fall of after som use.</t>
+  </si>
+  <si>
+    <t>Not possible to easilly switch of battery power. A manual toggle switch should be included in the battery power circuit.</t>
+  </si>
+  <si>
+    <t>Range stand does not provide sufficient stable "Game Start" indication. A slight foot-weight  change will be detected and cause a restart of the digital stop watch.</t>
+  </si>
+  <si>
+    <t>Stop watch accuracy not tested.</t>
+  </si>
+  <si>
+    <t>Sensitivity of the target hit detector are observed to be different.</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Use HAL_GetTick() to compare with the generated time …</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,16 +86,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,23 +135,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,57 +483,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="93" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>45524</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>45524</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>110</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45528</v>
+      </c>
+      <c r="E3" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674D9AF5-8B3F-42B1-A499-800A2BA920F5}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.453125" customWidth="1"/>
+    <col min="4" max="4" width="53.7265625" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>45528</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>